<commit_message>
data files up to date:18 juin
</commit_message>
<xml_diff>
--- a/raw data/2021/Corona (76) copy 344.xlsx
+++ b/raw data/2021/Corona (76) copy 344.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhou/Desktop/CovidCasesQC/raw data/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D587A5-8187-F74E-86EA-41E2E044F887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8634CF-7A37-2C44-9F6F-6FEDD2808C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="460" windowWidth="27320" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="460" windowWidth="27320" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -590,7 +590,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>19140</v>
+        <v>19138</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -662,7 +662,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>372478</v>
+        <v>372476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>